<commit_message>
Stable version - need to improve error and timing handling
</commit_message>
<xml_diff>
--- a/Requerimientos.xlsx
+++ b/Requerimientos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sponcino\Seba\proj-guardias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835CC6AA-AF3F-4B08-ABD1-145510FB6D94}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985BE48B-7992-4879-850B-786818902F9F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B261951C-FCB3-451E-AE7C-EEB08E1461AB}"/>
+    <workbookView xWindow="795" yWindow="795" windowWidth="18000" windowHeight="9360" xr2:uid="{B261951C-FCB3-451E-AE7C-EEB08E1461AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,17 +470,17 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="B2:D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -494,7 +494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -505,10 +505,10 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -519,10 +519,10 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -533,10 +533,10 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -547,10 +547,10 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -564,7 +564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -578,7 +578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -589,10 +589,10 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -606,7 +606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -620,7 +620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -634,7 +634,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -648,7 +648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -662,7 +662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -676,17 +676,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -725,9 +720,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -743,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -751,7 +746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>

</xml_diff>